<commit_message>
Dec update, Q3 start
</commit_message>
<xml_diff>
--- a/_data/FY23 Points Tracker Audit.xlsx
+++ b/_data/FY23 Points Tracker Audit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rymo/Repos/scconstructorschampionship/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6FD0AC-BB5C-8A46-8488-00C23A7DAC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2227CE-FB27-9C40-93A7-9D0E6469EEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22500" yWindow="-3540" windowWidth="22480" windowHeight="18000" xr2:uid="{22CDB5ED-B949-C944-AE1C-CD3953B56213}"/>
+    <workbookView xWindow="-22920" yWindow="-8660" windowWidth="22900" windowHeight="28300" xr2:uid="{22CDB5ED-B949-C944-AE1C-CD3953B56213}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1253,7 +1253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>John Szabo</t>
   </si>
@@ -1553,7 +1553,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1841,7 +1841,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1852,10 +1852,10 @@
   <dimension ref="A2:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G64" sqref="G64"/>
+      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2280,11 +2280,11 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ref="C24:I24" si="2">SUM(C26:C32)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
@@ -2292,11 +2292,11 @@
       </c>
       <c r="F24" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="2"/>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I24" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -2315,26 +2315,46 @@
         <v>8</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>15</v>
+      </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+      <c r="G26" s="1">
+        <v>4</v>
+      </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10</v>
+      </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="F27" s="1">
+        <v>5</v>
+      </c>
+      <c r="G27" s="1">
+        <v>5</v>
+      </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
@@ -2546,27 +2566,27 @@
       </c>
       <c r="D44" s="7">
         <f t="shared" si="4"/>
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="E44" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F44" s="7">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G44" s="7">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H44" s="7">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I44" s="7">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2588,7 +2608,9 @@
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
+      <c r="I46" s="16" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
@@ -2668,7 +2690,9 @@
       <c r="H51" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I51" s="16"/>
+      <c r="I51" s="16" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
@@ -2676,7 +2700,9 @@
       </c>
       <c r="B52" s="15"/>
       <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
+      <c r="D52" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="E52" s="16"/>
       <c r="F52" s="16" t="s">
         <v>33</v>
@@ -2719,25 +2745,25 @@
         <v>20</v>
       </c>
       <c r="C56" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D56" s="1">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E56" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F56" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G56" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H56" s="1">
         <v>17</v>
       </c>
       <c r="I56" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -2748,10 +2774,10 @@
         <v>8</v>
       </c>
       <c r="C57" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E57" s="1">
         <v>4</v>
@@ -2763,10 +2789,10 @@
         <v>12</v>
       </c>
       <c r="H57" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I57" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -2783,27 +2809,27 @@
       </c>
       <c r="D58" s="14">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E58" s="14">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F58" s="14">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G58" s="14">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H58" s="14">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I58" s="14">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2816,31 +2842,31 @@
       </c>
       <c r="C61" s="2">
         <f t="shared" ref="C61:I61" si="6">SUM(C4,C14,C24,C34,C44)</f>
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D61" s="2">
         <f t="shared" si="6"/>
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="E61" s="2">
         <f t="shared" si="6"/>
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F61" s="2">
         <f t="shared" si="6"/>
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="G61" s="2">
         <f t="shared" si="6"/>
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" si="6"/>
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" si="6"/>
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mar update, Q3 finish
</commit_message>
<xml_diff>
--- a/_data/FY23 Points Tracker Audit.xlsx
+++ b/_data/FY23 Points Tracker Audit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rymo/Repos/scconstructorschampionship/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2227CE-FB27-9C40-93A7-9D0E6469EEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B499B91-8053-584A-B1D4-21EB2F87C24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22920" yWindow="-8660" windowWidth="22900" windowHeight="28300" xr2:uid="{22CDB5ED-B949-C944-AE1C-CD3953B56213}"/>
+    <workbookView xWindow="-29940" yWindow="-5540" windowWidth="29280" windowHeight="24060" xr2:uid="{22CDB5ED-B949-C944-AE1C-CD3953B56213}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
+    <author>Ryan Morrissey</author>
   </authors>
   <commentList>
     <comment ref="B8" authorId="0" shapeId="0" xr:uid="{8D553F1C-29C6-444D-A472-EBB4055DCFDD}">
@@ -931,6 +932,158 @@
             <family val="2"/>
           </rPr>
           <t>https://netsuite-gbu.slack.com/archives/GEHVD04GK/p1666732759969909</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="1" shapeId="0" xr:uid="{781AE761-664F-644D-87EE-85ED3FB749AB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ryan Morrissey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">https://netsuite-gbu.slack.com/archives/GEHVD04GK/p1671744190888669
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://netsuite-gbu.slack.com/archives/GEHVD04GK/p1670612893066489</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="1" shapeId="0" xr:uid="{B9CD6BCD-EF51-D147-A657-B19EC55D0577}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ryan Morrissey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://netsuite-gbu.slack.com/archives/GEHVD04GK/p1671138247279569</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G28" authorId="1" shapeId="0" xr:uid="{6A8CF19A-3F4E-9B4C-B6B5-DFE2D0BA3B73}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ryan Morrissey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">https://netsuite-gbu.slack.com/archives/GEHVD04GK/p1671744190888669
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://netsuite-gbu.slack.com/archives/GEHVD04GK/p1671138247279569</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="1" shapeId="0" xr:uid="{E92E838B-13D0-4549-A8C8-7D1E3056A95F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ryan Morrissey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>New Feature Review</t>
         </r>
       </text>
     </comment>
@@ -1253,7 +1406,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>John Szabo</t>
   </si>
@@ -1553,7 +1706,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1841,7 +1994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1851,11 +2004,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A58CC0-BB18-5D4E-B714-747D0C991847}">
   <dimension ref="A2:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2102,7 +2255,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:I14" si="1">SUM(C16:C22)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
@@ -2215,9 +2368,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="1">
-        <v>-5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
         <v>-5</v>
@@ -2276,35 +2427,35 @@
       </c>
       <c r="B24" s="7">
         <f>SUM(B26:B32)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" ref="C24:I24" si="2">SUM(C26:C32)</f>
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -2314,46 +2465,58 @@
       <c r="A26" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="8">
+        <v>9</v>
+      </c>
       <c r="C26" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1">
-        <v>15</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="E26" s="1">
+        <v>39</v>
+      </c>
       <c r="F26" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G26" s="1">
-        <v>4</v>
-      </c>
-      <c r="H26" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="H26" s="1">
+        <v>26</v>
+      </c>
       <c r="I26" s="1">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="8">
+        <v>8</v>
+      </c>
       <c r="C27" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D27" s="1">
+        <v>20</v>
+      </c>
+      <c r="E27" s="1">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1">
         <v>10</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1">
-        <v>5</v>
-      </c>
       <c r="G27" s="1">
-        <v>5</v>
-      </c>
-      <c r="H27" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H27" s="1">
+        <v>13</v>
+      </c>
       <c r="I27" s="1">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -2361,11 +2524,17 @@
         <v>30</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="C28" s="1">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1">
+        <v>5</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
@@ -2378,9 +2547,15 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="G29" s="1">
+        <v>-10</v>
+      </c>
+      <c r="H29" s="1">
+        <v>-5</v>
+      </c>
+      <c r="I29" s="1">
+        <v>-5</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
@@ -2388,7 +2563,9 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1">
+        <v>23</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2558,35 +2735,35 @@
       </c>
       <c r="B44" s="7">
         <f>SUM(IF(NOT(ISBLANK(B46)),5,0),IF(NOT(ISBLANK(B47)),10,0),IF(NOT(ISBLANK(B48)),15,0),IF(NOT(ISBLANK(B49)),20,0),IF(NOT(ISBLANK(B51)),5,0),IF(NOT(ISBLANK(B52)),10,0),IF(NOT(ISBLANK(B53)),15,0),IF(NOT(ISBLANK(B54)),20,0),IF(NOT(ISBLANK(B58)),B58,0))</f>
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C44" s="7">
         <f t="shared" ref="C44:I44" si="4">SUM(IF(NOT(ISBLANK(C46)),5,0),IF(NOT(ISBLANK(C47)),10,0),IF(NOT(ISBLANK(C48)),15,0),IF(NOT(ISBLANK(C49)),20,0),IF(NOT(ISBLANK(C51)),5,0),IF(NOT(ISBLANK(C52)),10,0),IF(NOT(ISBLANK(C53)),15,0),IF(NOT(ISBLANK(C54)),20,0),IF(NOT(ISBLANK(C58)),C58,0))</f>
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D44" s="7">
         <f t="shared" si="4"/>
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="E44" s="7">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F44" s="7">
         <f t="shared" si="4"/>
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="G44" s="7">
         <f t="shared" si="4"/>
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="H44" s="7">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="I44" s="7">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2606,8 +2783,12 @@
       <c r="F46" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
+      <c r="G46" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="I46" s="16" t="s">
         <v>33</v>
       </c>
@@ -2620,7 +2801,9 @@
         <v>33</v>
       </c>
       <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
+      <c r="D47" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
       <c r="G47" s="16"/>
@@ -2674,7 +2857,9 @@
       <c r="B51" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C51" s="16"/>
+      <c r="C51" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="16" t="s">
         <v>33</v>
       </c>
@@ -2698,7 +2883,9 @@
       <c r="A52" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="15"/>
+      <c r="B52" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16" t="s">
         <v>33</v>
@@ -2707,7 +2894,9 @@
       <c r="F52" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G52" s="16"/>
+      <c r="G52" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="H52" s="16"/>
       <c r="I52" s="16"/>
     </row>
@@ -2742,28 +2931,28 @@
         <v>26</v>
       </c>
       <c r="B56" s="8">
+        <v>19</v>
+      </c>
+      <c r="C56" s="1">
+        <v>32</v>
+      </c>
+      <c r="D56" s="1">
+        <v>38</v>
+      </c>
+      <c r="E56" s="1">
+        <v>29</v>
+      </c>
+      <c r="F56" s="1">
+        <v>31</v>
+      </c>
+      <c r="G56" s="1">
+        <v>27</v>
+      </c>
+      <c r="H56" s="1">
+        <v>23</v>
+      </c>
+      <c r="I56" s="1">
         <v>20</v>
-      </c>
-      <c r="C56" s="1">
-        <v>24</v>
-      </c>
-      <c r="D56" s="1">
-        <v>34</v>
-      </c>
-      <c r="E56" s="1">
-        <v>24</v>
-      </c>
-      <c r="F56" s="1">
-        <v>21</v>
-      </c>
-      <c r="G56" s="1">
-        <v>20</v>
-      </c>
-      <c r="H56" s="1">
-        <v>17</v>
-      </c>
-      <c r="I56" s="1">
-        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -2771,28 +2960,28 @@
         <v>27</v>
       </c>
       <c r="B57" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C57" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D57" s="1">
+        <v>10</v>
+      </c>
+      <c r="E57" s="1">
         <v>6</v>
       </c>
-      <c r="E57" s="1">
-        <v>4</v>
-      </c>
       <c r="F57" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G57" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H57" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I57" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -2801,35 +2990,35 @@
       </c>
       <c r="B58" s="14">
         <f>B56+(2*B57)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C58" s="14">
         <f t="shared" ref="C58:I58" si="5">C56+(2*C57)</f>
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D58" s="14">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E58" s="14">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F58" s="14">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G58" s="14">
         <f t="shared" si="5"/>
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H58" s="14">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="I58" s="14">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2838,35 +3027,35 @@
       </c>
       <c r="B61" s="2">
         <f>SUM(B4,B14,B24,B34,B44)</f>
-        <v>411</v>
+        <v>439</v>
       </c>
       <c r="C61" s="2">
         <f t="shared" ref="C61:I61" si="6">SUM(C4,C14,C24,C34,C44)</f>
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="D61" s="2">
         <f t="shared" si="6"/>
-        <v>256</v>
+        <v>331</v>
       </c>
       <c r="E61" s="2">
         <f t="shared" si="6"/>
-        <v>164</v>
+        <v>225</v>
       </c>
       <c r="F61" s="2">
         <f t="shared" si="6"/>
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="G61" s="2">
         <f t="shared" si="6"/>
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" si="6"/>
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" si="6"/>
-        <v>171</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>